<commit_message>
latex started first section
</commit_message>
<xml_diff>
--- a/_memoria/01_Introducció/projectPlanning.xlsx
+++ b/_memoria/01_Introducció/projectPlanning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Primer estudi superficial de l'API</t>
   </si>
@@ -30,33 +30,15 @@
     <t>Preparació de la presentació</t>
   </si>
   <si>
-    <t>Decissió i estudi de les tecnologies a utilitzar per l'aplicació web</t>
-  </si>
-  <si>
     <t>9.5</t>
   </si>
   <si>
     <t>10.5</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>Decissió tipus d'aplicació a implementar i definició de l'estructura del projecte</t>
-  </si>
-  <si>
     <t>FASE DEL PROJECTE / SETMANA</t>
   </si>
   <si>
-    <t>Propostes de projecte per futurs estudiants i estudi de la API</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
     <t>Febrer 2016</t>
   </si>
   <si>
@@ -103,13 +85,22 @@
   </si>
   <si>
     <t>Preparació de la defensa del projecte</t>
+  </si>
+  <si>
+    <t>Propostes de projecte per futurs estudiants i estudi de l'API</t>
+  </si>
+  <si>
+    <t>Decisió i estudi de les tecnologies a utilitzar per l'aplicació web</t>
+  </si>
+  <si>
+    <t>Decisió tipus d'aplicació a implementar i definició de l'estructura</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +133,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,9 +260,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -282,6 +277,16 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,106 +585,106 @@
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="30" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="84.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="20">
+        <v>6</v>
+      </c>
+      <c r="B1" s="19">
         <v>42450</v>
       </c>
-      <c r="C1" s="20">
+      <c r="C1" s="19">
         <v>42457</v>
       </c>
-      <c r="D1" s="21">
+      <c r="D1" s="20">
         <v>42464</v>
       </c>
-      <c r="E1" s="21">
+      <c r="E1" s="20">
         <v>42471</v>
       </c>
-      <c r="F1" s="21">
+      <c r="F1" s="20">
         <v>42478</v>
       </c>
-      <c r="G1" s="21">
+      <c r="G1" s="20">
         <v>42485</v>
       </c>
-      <c r="H1" s="20">
+      <c r="H1" s="19">
         <v>42492</v>
       </c>
-      <c r="I1" s="20">
+      <c r="I1" s="19">
         <v>42499</v>
       </c>
-      <c r="J1" s="20">
+      <c r="J1" s="19">
         <v>42506</v>
       </c>
-      <c r="K1" s="20">
+      <c r="K1" s="19">
         <v>42513</v>
       </c>
-      <c r="L1" s="21">
+      <c r="L1" s="20">
         <v>42520</v>
       </c>
-      <c r="M1" s="21">
+      <c r="M1" s="20">
         <v>42527</v>
       </c>
-      <c r="N1" s="21">
+      <c r="N1" s="20">
         <v>42534</v>
       </c>
-      <c r="O1" s="21">
+      <c r="O1" s="20">
         <v>42541</v>
       </c>
-      <c r="P1" s="21">
+      <c r="P1" s="20">
         <v>42548</v>
       </c>
-      <c r="Q1" s="20">
+      <c r="Q1" s="19">
         <v>42555</v>
       </c>
-      <c r="R1" s="20">
+      <c r="R1" s="19">
         <v>42562</v>
       </c>
-      <c r="S1" s="20">
+      <c r="S1" s="19">
         <v>42569</v>
       </c>
-      <c r="T1" s="20">
+      <c r="T1" s="19">
         <v>42576</v>
       </c>
-      <c r="U1" s="21">
+      <c r="U1" s="20">
         <v>42583</v>
       </c>
-      <c r="V1" s="21">
+      <c r="V1" s="20">
         <v>42590</v>
       </c>
-      <c r="W1" s="21">
+      <c r="W1" s="20">
         <v>42597</v>
       </c>
-      <c r="X1" s="21">
+      <c r="X1" s="20">
         <v>42604</v>
       </c>
-      <c r="Y1" s="20">
+      <c r="Y1" s="19">
         <v>42611</v>
       </c>
-      <c r="Z1" s="20">
+      <c r="Z1" s="19">
         <v>42618</v>
       </c>
-      <c r="AA1" s="20">
+      <c r="AA1" s="19">
         <v>42625</v>
       </c>
-      <c r="AB1" s="20">
+      <c r="AB1" s="19">
         <v>42632</v>
       </c>
-      <c r="AC1" s="20">
+      <c r="AC1" s="19">
         <v>42639</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="33" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4">
@@ -716,8 +721,8 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="33" customHeight="1">
-      <c r="A3" s="18" t="s">
-        <v>9</v>
+      <c r="A3" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -753,8 +758,8 @@
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" ht="33" customHeight="1">
-      <c r="A4" s="18" t="s">
-        <v>4</v>
+      <c r="A4" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -783,13 +788,13 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="Q4" s="7">
         <v>7</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="S4" s="7">
         <v>8</v>
@@ -806,32 +811,36 @@
       <c r="AC4" s="5"/>
     </row>
     <row r="5" spans="1:29" ht="33" customHeight="1">
-      <c r="A5" s="18" t="s">
-        <v>11</v>
+      <c r="A5" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="7">
+      <c r="H5" s="4">
         <v>3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4</v>
+      </c>
+      <c r="J5" s="24">
+        <v>4.5</v>
+      </c>
+      <c r="K5" s="24">
+        <v>5</v>
+      </c>
+      <c r="L5" s="24">
+        <v>5.5</v>
+      </c>
+      <c r="M5" s="24">
+        <v>6</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -840,26 +849,26 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="4">
-        <v>4</v>
-      </c>
-      <c r="V5" s="4">
-        <v>5</v>
-      </c>
-      <c r="W5" s="4">
-        <v>6</v>
-      </c>
-      <c r="X5" s="4">
+      <c r="U5" s="21"/>
+      <c r="V5" s="24">
+        <v>6.5</v>
+      </c>
+      <c r="W5" s="24">
         <v>7</v>
       </c>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
+      <c r="X5" s="24">
+        <v>7.5</v>
+      </c>
+      <c r="Y5" s="24">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="21"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
     </row>
     <row r="6" spans="1:29" ht="33" customHeight="1">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="5"/>
@@ -899,26 +908,28 @@
       <c r="T6" s="4">
         <v>9</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="7" t="s">
+      <c r="U6" s="22"/>
+      <c r="V6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" s="7">
+        <v>10</v>
+      </c>
+      <c r="X6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="X6" s="7">
-        <v>10</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>6</v>
+      <c r="Y6" s="7">
+        <v>11</v>
       </c>
       <c r="Z6" s="7">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
     </row>
     <row r="7" spans="1:29" ht="33" customHeight="1">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="5"/>
@@ -965,8 +976,8 @@
       <c r="AC7" s="5"/>
     </row>
     <row r="8" spans="1:29" ht="33" customHeight="1">
-      <c r="A8" s="19" t="s">
-        <v>28</v>
+      <c r="A8" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1010,6 +1021,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="V6:Z6 P4:S4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1018,103 +1032,103 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="8" width="12.28515625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="8" width="11.28515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.75" customHeight="1">
+    <row r="1" spans="1:8" ht="33" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="33" customHeight="1">
+      <c r="A2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A3" s="15" t="s">
-        <v>24</v>
+    <row r="3" spans="1:8" ht="33" customHeight="1">
+      <c r="A3" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="16"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A4" s="15" t="s">
-        <v>21</v>
+    <row r="4" spans="1:8" ht="33" customHeight="1">
+      <c r="A4" s="23" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A5" s="15" t="s">
-        <v>22</v>
+    <row r="5" spans="1:8" ht="33" customHeight="1">
+      <c r="A5" s="23" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A6" s="15" t="s">
-        <v>23</v>
+    <row r="6" spans="1:8" ht="33" customHeight="1">
+      <c r="A6" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="29.25" customHeight="1">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:8" ht="33" customHeight="1">
+      <c r="A7" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1"/>
@@ -1123,7 +1137,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="17"/>
+      <c r="H7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>